<commit_message>
class work for driver
</commit_message>
<xml_diff>
--- a/Lab0x04/Romi_Pinout.xlsx
+++ b/Lab0x04/Romi_Pinout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noahtanner/Desktop/Fall 2023/ME 405/Lab0x04/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F40018-DB90-F542-B33B-18558A960C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058E58B3-662A-B847-96E2-D05A7651D255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="500" windowWidth="16800" windowHeight="19340" xr2:uid="{5E2C103A-F690-4841-AD40-264B3F1C0F2F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16800" windowHeight="19340" xr2:uid="{5E2C103A-F690-4841-AD40-264B3F1C0F2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="51">
   <si>
     <t>Item</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>Yellow</t>
+  </si>
+  <si>
+    <t>Romi Driver Logic Table</t>
+  </si>
+  <si>
+    <t>Power Distribution Board Logic Table</t>
   </si>
 </sst>
 </file>
@@ -236,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -248,6 +254,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -265,6 +274,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>36531</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>30251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>455631</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>137064</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B51114C0-8094-088A-87D4-07B6B1335720}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7656531" y="230026"/>
+          <a:ext cx="6212583" cy="1505240"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>14269</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>57080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>466046</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>46455</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF6686FD-F160-BA32-2C17-1210F7115615}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7634269" y="2454383"/>
+          <a:ext cx="6245260" cy="1987128"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -564,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3AB7D52-B086-6E45-9AD2-06C2926AC8EC}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -575,7 +677,7 @@
     <col min="1" max="1" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -600,8 +702,12 @@
       <c r="H1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="5"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -627,7 +733,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>18</v>
@@ -651,7 +757,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>19</v>
@@ -675,7 +781,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>17</v>
@@ -699,7 +805,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>18</v>
@@ -723,7 +829,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>19</v>
@@ -747,7 +853,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -756,7 +862,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -780,7 +886,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
@@ -801,8 +907,13 @@
       <c r="H10" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
@@ -824,7 +935,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
@@ -846,7 +957,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -855,7 +966,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
@@ -878,7 +989,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -887,7 +998,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>45</v>
       </c>
@@ -911,6 +1022,11 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J10:L10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added register read and write method for calibration coeffs
</commit_message>
<xml_diff>
--- a/Lab0x04/Romi_Pinout.xlsx
+++ b/Lab0x04/Romi_Pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noahtanner/Desktop/Fall 2023/ME 405/Lab0x04/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058E58B3-662A-B847-96E2-D05A7651D255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0AA6DD-A578-A04F-A0A4-BCB6675FD458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="16800" windowHeight="19340" xr2:uid="{5E2C103A-F690-4841-AD40-264B3F1C0F2F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="64">
   <si>
     <t>Item</t>
   </si>
@@ -189,6 +189,45 @@
   </si>
   <si>
     <t>Power Distribution Board Logic Table</t>
+  </si>
+  <si>
+    <t>STM (D)</t>
+  </si>
+  <si>
+    <t>PWM8/3</t>
+  </si>
+  <si>
+    <t>PWM8/4</t>
+  </si>
+  <si>
+    <t>D9 [ PWM8/2 ]</t>
+  </si>
+  <si>
+    <t>PWM4/3</t>
+  </si>
+  <si>
+    <t>PWM4/4</t>
+  </si>
+  <si>
+    <t>PWM4/2</t>
+  </si>
+  <si>
+    <t>D7 [ PWM1/1 ]</t>
+  </si>
+  <si>
+    <t>D8 [ PWM1/2 ]</t>
+  </si>
+  <si>
+    <t>D5 [ PWM3/1 ]</t>
+  </si>
+  <si>
+    <t>D4 [ PWM3/2 ]</t>
+  </si>
+  <si>
+    <t>BNO055 Modes</t>
+  </si>
+  <si>
+    <t>BNO055 Address</t>
   </si>
 </sst>
 </file>
@@ -325,15 +364,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>14269</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>57080</xdr:rowOff>
+      <xdr:colOff>43804</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>71847</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>466046</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>46455</xdr:rowOff>
+      <xdr:colOff>495581</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>61222</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -356,8 +395,96 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7634269" y="2454383"/>
-          <a:ext cx="6245260" cy="1987128"/>
+          <a:off x="7885316" y="2139289"/>
+          <a:ext cx="6240614" cy="2056817"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>29534</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>44304</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>812210</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>62763</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{512CBF9A-3542-F447-A0DC-D89069CF6B5B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14486860" y="457792"/>
+          <a:ext cx="4917559" cy="3533111"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>22477</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>44303</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>790222</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>10421</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A24854A6-411C-BA2E-8E8E-4DBE80A4ACD9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14458144" y="4341136"/>
+          <a:ext cx="4895245" cy="1603007"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -666,18 +793,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3AB7D52-B086-6E45-9AD2-06C2926AC8EC}">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="146" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -697,9 +825,12 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="5" t="s">
@@ -707,7 +838,7 @@
       </c>
       <c r="K1" s="5"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -727,13 +858,20 @@
         <v>24</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="R2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="S2" s="5"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>18</v>
@@ -751,13 +889,16 @@
         <v>25</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>19</v>
@@ -775,13 +916,16 @@
         <v>26</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>17</v>
@@ -799,13 +943,16 @@
         <v>27</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>18</v>
@@ -823,13 +970,16 @@
         <v>29</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>19</v>
@@ -847,22 +997,25 @@
         <v>28</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -880,13 +1033,16 @@
         <v>36</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
@@ -902,9 +1058,12 @@
         <v>37</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>48</v>
       </c>
       <c r="J10" s="5" t="s">
@@ -913,7 +1072,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
@@ -929,13 +1088,16 @@
         <v>38</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
@@ -951,13 +1113,16 @@
         <v>39</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="I12" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -966,7 +1131,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
@@ -988,8 +1153,14 @@
       <c r="G14" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -997,8 +1168,10 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>45</v>
       </c>
@@ -1020,11 +1193,25 @@
       <c r="G16" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="H16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="18:19" x14ac:dyDescent="0.2">
+      <c r="R21" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="S21" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="J10:L10"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="R21:S21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
back at it. IMU class setup and updating reg addresses
</commit_message>
<xml_diff>
--- a/Lab0x04/Romi_Pinout.xlsx
+++ b/Lab0x04/Romi_Pinout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noahtanner/Desktop/Fall 2023/ME 405/Lab0x04/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0AA6DD-A578-A04F-A0A4-BCB6675FD458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64865D5D-1AFD-9244-B858-7584BA3FA7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="16800" windowHeight="19340" xr2:uid="{5E2C103A-F690-4841-AD40-264B3F1C0F2F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19340" xr2:uid="{5E2C103A-F690-4841-AD40-264B3F1C0F2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="119">
   <si>
     <t>Item</t>
   </si>
@@ -77,9 +77,6 @@
     <t>ch_3</t>
   </si>
   <si>
-    <t>ch_4</t>
-  </si>
-  <si>
     <t>ch_2</t>
   </si>
   <si>
@@ -122,6 +119,9 @@
     <t>PB8</t>
   </si>
   <si>
+    <t>PB0</t>
+  </si>
+  <si>
     <t>PB7</t>
   </si>
   <si>
@@ -224,17 +224,182 @@
     <t>D4 [ PWM3/2 ]</t>
   </si>
   <si>
-    <t>BNO055 Modes</t>
-  </si>
-  <si>
-    <t>BNO055 Address</t>
+    <t>OP Modes</t>
+  </si>
+  <si>
+    <t>I2C Address</t>
+  </si>
+  <si>
+    <t>Ang Velocity</t>
+  </si>
+  <si>
+    <t>P .34</t>
+  </si>
+  <si>
+    <t>Tab 3-5</t>
+  </si>
+  <si>
+    <t>Tab 4-7</t>
+  </si>
+  <si>
+    <t>Tab 3-27</t>
+  </si>
+  <si>
+    <t>P. 90</t>
+  </si>
+  <si>
+    <t>P. 21</t>
+  </si>
+  <si>
+    <t>BNO055 Relevant Pages / Tables</t>
+  </si>
+  <si>
+    <t>Vin</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>SCL</t>
+  </si>
+  <si>
+    <t>3V3</t>
+  </si>
+  <si>
+    <t>CN6 5</t>
+  </si>
+  <si>
+    <t>CN6 4</t>
+  </si>
+  <si>
+    <t>PC1</t>
+  </si>
+  <si>
+    <t>PC0</t>
+  </si>
+  <si>
+    <t>I2C3_SDA</t>
+  </si>
+  <si>
+    <t>I2C3_SCL</t>
+  </si>
+  <si>
+    <t>CN8 2</t>
+  </si>
+  <si>
+    <t>CN8 1</t>
+  </si>
+  <si>
+    <t>VCC</t>
+  </si>
+  <si>
+    <t>QTR 3</t>
+  </si>
+  <si>
+    <t>QTR 4</t>
+  </si>
+  <si>
+    <t>QTR 5</t>
+  </si>
+  <si>
+    <t>QTR 6</t>
+  </si>
+  <si>
+    <t>QTR 7</t>
+  </si>
+  <si>
+    <t>QTR 8</t>
+  </si>
+  <si>
+    <t>QTR 9</t>
+  </si>
+  <si>
+    <t>5V</t>
+  </si>
+  <si>
+    <t>CN6 2</t>
+  </si>
+  <si>
+    <t>CN6 3</t>
+  </si>
+  <si>
+    <t>PA5</t>
+  </si>
+  <si>
+    <t>CN5 6</t>
+  </si>
+  <si>
+    <t>ENA</t>
+  </si>
+  <si>
+    <t>ENB</t>
+  </si>
+  <si>
+    <t>CN8 6</t>
+  </si>
+  <si>
+    <t>CN8 5</t>
+  </si>
+  <si>
+    <t>CN8 4</t>
+  </si>
+  <si>
+    <t>CN8 3</t>
+  </si>
+  <si>
+    <t>AN_A0</t>
+  </si>
+  <si>
+    <t>AN_A1</t>
+  </si>
+  <si>
+    <t>AN_A2</t>
+  </si>
+  <si>
+    <t>AN_A3</t>
+  </si>
+  <si>
+    <t>AN_D1</t>
+  </si>
+  <si>
+    <t>AN_D0</t>
+  </si>
+  <si>
+    <t>CN9 2</t>
+  </si>
+  <si>
+    <t>CN9 1</t>
+  </si>
+  <si>
+    <t>PA2</t>
+  </si>
+  <si>
+    <t>PA3</t>
+  </si>
+  <si>
+    <t>PA0</t>
+  </si>
+  <si>
+    <t>PA1</t>
+  </si>
+  <si>
+    <t>PA4</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Black</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -242,8 +407,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -268,6 +446,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -281,11 +471,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -296,6 +487,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -320,13 +518,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>36531</xdr:colOff>
+      <xdr:colOff>123369</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>30251</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>455631</xdr:colOff>
+      <xdr:colOff>542469</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>137064</xdr:rowOff>
     </xdr:to>
@@ -351,8 +549,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7656531" y="230026"/>
-          <a:ext cx="6212583" cy="1505240"/>
+          <a:off x="7949608" y="236490"/>
+          <a:ext cx="6193801" cy="1550489"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -364,13 +562,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>43804</xdr:colOff>
+      <xdr:colOff>141496</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>71847</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>495581</xdr:colOff>
+      <xdr:colOff>593273</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>61222</xdr:rowOff>
     </xdr:to>
@@ -395,8 +593,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7885316" y="2139289"/>
-          <a:ext cx="6240614" cy="2056817"/>
+          <a:off x="7967735" y="2134240"/>
+          <a:ext cx="6226478" cy="2051768"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -407,23 +605,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>29534</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>44304</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>387058</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>24284</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>812210</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>62763</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>33728</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>153073</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{512CBF9A-3542-F447-A0DC-D89069CF6B5B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8083D51-0EB5-5302-A423-D96A73143AE2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -439,8 +637,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14486860" y="457792"/>
-          <a:ext cx="4917559" cy="3533111"/>
+          <a:off x="4692358" y="5713884"/>
+          <a:ext cx="3177270" cy="2363989"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -451,23 +649,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>22477</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>44303</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>100507</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>162915</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>790222</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>10421</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>258932</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>26356</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
+        <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A24854A6-411C-BA2E-8E8E-4DBE80A4ACD9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C362B1F3-636E-576D-B305-C18760815550}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -483,8 +681,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14458144" y="4341136"/>
-          <a:ext cx="4895245" cy="1603007"/>
+          <a:off x="100507" y="5649315"/>
+          <a:ext cx="4463725" cy="4130641"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -793,19 +991,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3AB7D52-B086-6E45-9AD2-06C2926AC8EC}">
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="146" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.1640625" customWidth="1"/>
     <col min="7" max="7" width="13.83203125" customWidth="1"/>
+    <col min="18" max="18" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -813,7 +1012,7 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -833,17 +1032,17 @@
       <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="5"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K1" s="6"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -855,7 +1054,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>52</v>
@@ -863,30 +1062,31 @@
       <c r="H2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="R2" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="S2" s="5"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R2" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>53</v>
@@ -894,26 +1094,35 @@
       <c r="H3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R3" t="s">
+        <v>62</v>
+      </c>
+      <c r="S3" t="s">
+        <v>70</v>
+      </c>
+      <c r="T3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>54</v>
@@ -921,26 +1130,35 @@
       <c r="H4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R4" t="s">
+        <v>63</v>
+      </c>
+      <c r="S4" t="s">
+        <v>69</v>
+      </c>
+      <c r="T4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>55</v>
@@ -948,23 +1166,32 @@
       <c r="H5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R5" t="s">
+        <v>64</v>
+      </c>
+      <c r="S5" t="s">
+        <v>65</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>29</v>
@@ -975,23 +1202,23 @@
       <c r="H6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>28</v>
@@ -1002,11 +1229,11 @@
       <c r="H7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1015,19 +1242,21 @@
       <c r="F8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>36</v>
@@ -1038,21 +1267,23 @@
       <c r="H9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>37</v>
@@ -1063,26 +1294,28 @@
       <c r="H10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>38</v>
@@ -1093,21 +1326,23 @@
       <c r="H11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>39</v>
@@ -1118,11 +1353,11 @@
       <c r="H12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1131,12 +1366,12 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>10</v>
@@ -1148,71 +1383,348 @@
         <v>10</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="B15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="18:19" x14ac:dyDescent="0.2">
-      <c r="R21" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="S21" s="5"/>
+      <c r="B19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R31" s="6"/>
+      <c r="S31" s="6"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I40" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="J10:L10"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="R31:S31"/>
+    <mergeCell ref="R2:T2"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>